<commit_message>
start working at Tarife
</commit_message>
<xml_diff>
--- a/structura.xlsx
+++ b/structura.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Clinet" sheetId="3" r:id="rId3"/>
     <sheet name="Antrenor" sheetId="2" r:id="rId4"/>
     <sheet name="Director" sheetId="4" r:id="rId5"/>
+    <sheet name="Tarif" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="25">
   <si>
     <t>director</t>
   </si>
@@ -80,6 +81,24 @@
   </si>
   <si>
     <t>Galerie</t>
+  </si>
+  <si>
+    <t>Abonament sala</t>
+  </si>
+  <si>
+    <t>Antrenor</t>
+  </si>
+  <si>
+    <t>dropdown - standard, de familie</t>
+  </si>
+  <si>
+    <t>dropdown - nume antrenori</t>
+  </si>
+  <si>
+    <t>Abonament sauna</t>
+  </si>
+  <si>
+    <t>Sedinta sauna</t>
   </si>
 </sst>
 </file>
@@ -124,7 +143,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -142,16 +161,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -433,7 +442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -843,4 +852,45 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>